<commit_message>
add Construction to use ImpactIndicator and ConstructionItem for cost and environmental impact calculation during construction
</commit_message>
<xml_diff>
--- a/sanitation/data/lca_data/_construction_item.xlsx
+++ b/sanitation/data/lca_data/_construction_item.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/data/lca_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B51E576A-4B3A-2E43-A7FE-7ADC7EC244D0}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{782A01B8-F17C-4548-81F5-A3BC7B2B1950}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="3760" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="11160" yWindow="3740" windowWidth="27240" windowHeight="16440" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="GWP" sheetId="1" r:id="rId2"/>
+    <sheet name="Eutrophication" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="30">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -116,6 +117,15 @@
   </si>
   <si>
     <t>kg CO2-eq</t>
+  </si>
+  <si>
+    <t>g N</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>price_unit</t>
   </si>
 </sst>
 </file>
@@ -509,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,7 +532,7 @@
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -532,8 +542,14 @@
       <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -544,7 +560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -555,7 +571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -566,7 +582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -577,7 +593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -588,7 +604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -599,7 +615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -610,7 +626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -621,7 +637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -632,7 +648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -643,7 +659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -663,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28627DAA-889C-6942-A3B5-3C8A993554C1}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -959,4 +975,278 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BA73E1-0EB2-7B4F-9241-A5B8DBA36260}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6">
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="D2" s="6">
+        <v>7.1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7">
+        <v>12.8</v>
+      </c>
+      <c r="D4" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="E4" s="7">
+        <v>13.899999999999999</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6">
+        <v>45.3</v>
+      </c>
+      <c r="D9" s="6">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E9" s="6">
+        <v>57</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="E10" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>23.299999999999997</v>
+      </c>
+      <c r="E11" s="6">
+        <v>33.5</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1972</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1862</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2082</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add construction design to PitLatrine
</commit_message>
<xml_diff>
--- a/sanitation/data/lca_data/_construction_item.xlsx
+++ b/sanitation/data/lca_data/_construction_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/data/lca_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{782A01B8-F17C-4548-81F5-A3BC7B2B1950}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3EF2BD76-D1AC-5840-9BB1-01D94DA885F0}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="3740" windowWidth="27240" windowHeight="16440" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="11160" yWindow="3740" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="30">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>Bricks</t>
-  </si>
-  <si>
     <t>Cement</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>price_unit</t>
+  </si>
+  <si>
+    <t>Brick</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,129 +534,129 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -664,10 +664,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +680,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,33 +691,34 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>info!A2</f>
+        <v>Excavation</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2" s="6">
         <v>0.53</v>
@@ -736,11 +737,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" t="str">
+        <f>info!A3</f>
+        <v>Brick</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7">
         <v>0.28000000000000003</v>
@@ -759,11 +761,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" t="str">
+        <f>info!A4</f>
+        <v>Cement</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7">
         <v>1.08</v>
@@ -782,11 +785,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>23</v>
+      <c r="A5" t="str">
+        <f>info!A5</f>
+        <v>Concrete</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4">
         <v>300</v>
@@ -805,11 +809,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" t="str">
+        <f>info!A6</f>
+        <v>Gravel</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6">
         <v>1.4999999999999999E-2</v>
@@ -828,11 +833,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="A7" t="str">
+        <f>info!A7</f>
+        <v>Plastic</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6">
         <v>1.97</v>
@@ -851,11 +857,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
+      <c r="A8" t="str">
+        <f>info!A8</f>
+        <v>Sand</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="6">
         <v>1.2E-2</v>
@@ -874,11 +881,12 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
+      <c r="A9" t="str">
+        <f>info!A9</f>
+        <v>StainlessSteel</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="6">
         <v>4.33</v>
@@ -897,11 +905,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
+      <c r="A10" t="str">
+        <f>info!A10</f>
+        <v>StainlessSteelSheet</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="6">
         <v>0.65</v>
@@ -920,11 +929,12 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" t="str">
+        <f>info!A11</f>
+        <v>Steel</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6">
         <v>2.5499999999999998</v>
@@ -943,11 +953,12 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
+      <c r="A12" t="str">
+        <f>info!A12</f>
+        <v>Wood</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="6">
         <v>197</v>
@@ -981,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BA73E1-0EB2-7B4F-9241-A5B8DBA36260}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,33 +1004,34 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
+      <c r="A2" t="str">
+        <f>info!A2</f>
+        <v>Excavation</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6">
         <v>7.3000000000000007</v>
@@ -1038,11 +1050,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" t="str">
+        <f>info!A3</f>
+        <v>Brick</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7">
         <v>4.8000000000000007</v>
@@ -1061,11 +1074,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" t="str">
+        <f>info!A4</f>
+        <v>Cement</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7">
         <v>12.8</v>
@@ -1084,11 +1098,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>23</v>
+      <c r="A5" t="str">
+        <f>info!A5</f>
+        <v>Concrete</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1101,11 +1116,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" t="str">
+        <f>info!A6</f>
+        <v>Gravel</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1118,11 +1134,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="A7" t="str">
+        <f>info!A7</f>
+        <v>Plastic</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1135,11 +1152,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
+      <c r="A8" t="str">
+        <f>info!A8</f>
+        <v>Sand</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1152,11 +1170,12 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
+      <c r="A9" t="str">
+        <f>info!A9</f>
+        <v>StainlessSteel</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="6">
         <v>45.3</v>
@@ -1175,11 +1194,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
+      <c r="A10" t="str">
+        <f>info!A10</f>
+        <v>StainlessSteelSheet</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6">
         <v>8.5</v>
@@ -1198,11 +1218,12 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" t="str">
+        <f>info!A11</f>
+        <v>Steel</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6">
         <v>27.5</v>
@@ -1221,11 +1242,12 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
+      <c r="A12" t="str">
+        <f>info!A12</f>
+        <v>Wood</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="6">
         <v>1972</v>

</xml_diff>